<commit_message>
nov - dec12 titrator data analysis and plots
</commit_message>
<xml_diff>
--- a/Water_Chemistry/data/Titrator/TrisCalibration.xlsx
+++ b/Water_Chemistry/data/Titrator/TrisCalibration.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Shelly/Documents/GitHub/P_generosa/Water_Chemistry/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Shelly/Documents/GitHub/P_generosa/Water_Chemistry/data/Titrator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88C133FB-4D60-BC4E-9D05-D66A353E61D0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05DB47D1-0C53-864A-96B4-9538003D5940}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5280" yWindow="640" windowWidth="22420" windowHeight="13940" activeTab="6" xr2:uid="{CFC1D0D6-766B-0649-B317-8AE9A7B8F3ED}"/>
+    <workbookView xWindow="3180" yWindow="640" windowWidth="22420" windowHeight="13940" activeTab="7" xr2:uid="{CFC1D0D6-766B-0649-B317-8AE9A7B8F3ED}"/>
   </bookViews>
   <sheets>
     <sheet name="Nov7" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="Nov28" sheetId="7" r:id="rId5"/>
     <sheet name="Dec05" sheetId="5" r:id="rId6"/>
     <sheet name="Dec12" sheetId="6" r:id="rId7"/>
+    <sheet name="Dec19" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -9824,7 +9825,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B468DAD7-B567-8541-A260-F7BF4EC09EDA}">
   <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
@@ -10068,4 +10069,16 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{961E40E5-88D5-6643-A352-38B8186F0DAB}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>